<commit_message>
Formatage de l'en-tête de la progression pour impression pour l'inspecteur académique
</commit_message>
<xml_diff>
--- a/1ere_NSI/z.Progression1NSI_MBR_02.xlsx
+++ b/1ere_NSI/z.Progression1NSI_MBR_02.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcbiver/Documents/01_Prof/40_1ere_NSI/10.Progression/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcbiver/Documents/01_Prof/10_Forge_AEIF/_Forge/1ere_NSI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8988333-E9C7-C94A-9101-81B093C97F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC80DD9-1118-9641-B0A5-02D5610CEA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressionMBR" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Programme!$A$1:$H$994</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProgressionMBR!$A$1:$F$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ProgressionMBR_PRINT!$A$1:$E$46</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">ProgressionMBR_PRINT!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -1114,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1196,24 +1197,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1492,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XEV45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
@@ -1517,10 +1500,10 @@
       <c r="B1" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -18120,25 +18103,25 @@
       <c r="AMC22" s="19"/>
       <c r="AMD22" s="19"/>
     </row>
-    <row r="23" spans="1:1018 16375:16376" s="32" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="28">
+    <row r="23" spans="1:1018 16375:16376" s="7" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10">
         <v>45320</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="11">
         <v>22</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="XEU23" s="33"/>
-      <c r="XEV23" s="33"/>
+      <c r="F23" s="6"/>
+      <c r="XEU23" s="19"/>
+      <c r="XEV23" s="19"/>
     </row>
     <row r="24" spans="1:1018 16375:16376" s="7" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
@@ -23580,22 +23563,22 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="29" t="s">
         <v>161</v>
       </c>
     </row>
@@ -23640,22 +23623,22 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.15">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="29" t="s">
         <v>161</v>
       </c>
     </row>
@@ -23694,9 +23677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8AD568-4811-1342-9396-688F6B1D2247}">
   <dimension ref="A1:XEU45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.19921875" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -23721,7 +23704,7 @@
       <c r="C1" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -40326,27 +40309,27 @@
       <c r="AMB22" s="19"/>
       <c r="AMC22" s="19"/>
     </row>
-    <row r="23" spans="1:1017 16374:16375" s="32" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="28">
+    <row r="23" spans="1:1017 16374:16375" s="7" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="10">
         <v>45320</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="11">
         <v>22</v>
       </c>
-      <c r="C23" s="29" t="str">
+      <c r="C23" s="11" t="str">
         <f>ProgressionMBR!C23</f>
         <v>Tables</v>
       </c>
-      <c r="D23" s="29" t="str">
+      <c r="D23" s="11" t="str">
         <f>ProgressionMBR!D23</f>
         <v>ALG_1, DTT_2, DTT_3, DTT_4</v>
       </c>
-      <c r="E23" s="30" t="str">
+      <c r="E23" s="12" t="str">
         <f>ProgressionMBR!E23</f>
         <v>S'appuyant sur le chargement de données depuis les fichiers CSV, retour sur la notion de tableaux: calculs de sommes, de moyennes; recherche d'un élément; recherche de doublons; tri - introduction de sort() et sorted(); fusion de tables.</v>
       </c>
-      <c r="XET23" s="33"/>
-      <c r="XEU23" s="33"/>
+      <c r="XET23" s="19"/>
+      <c r="XEU23" s="19"/>
     </row>
     <row r="24" spans="1:1017 16374:16375" s="7" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
@@ -44776,11 +44759,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E46" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <pageMargins left="0" right="0" top="1" bottom="0.5" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Bold Italic"&amp;14Progression NSI Première 2019-2020</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader>&amp;L&amp;"Arial Bold Italic,Bold Italic"&amp;14Marc Biver&amp;C&amp;"Arial Bold Italic,Bold Italic"&amp;16Progression 2nde SNT 2023-24
+&amp;R&amp;"Arial Bold Italic,Bold Italic"&amp;14&amp;D</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -44795,14 +44779,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11" style="38"/>
+    <col min="2" max="2" width="11" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="30" t="s">
         <v>234</v>
       </c>
     </row>
@@ -44810,8 +44794,8 @@
       <c r="A2" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="38" t="str">
-        <f>IF(C2&lt;&gt;A2,"X","")</f>
+      <c r="B2" s="32" t="str">
+        <f t="shared" ref="B2:B31" si="0">IF(C2&lt;&gt;A2,"X","")</f>
         <v/>
       </c>
       <c r="C2" t="s">
@@ -44822,8 +44806,8 @@
       <c r="A3" t="s">
         <v>203</v>
       </c>
-      <c r="B3" s="38" t="str">
-        <f>IF(C3&lt;&gt;A3,"X","")</f>
+      <c r="B3" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C3" t="s">
@@ -44834,8 +44818,8 @@
       <c r="A4" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="38" t="str">
-        <f>IF(C4&lt;&gt;A4,"X","")</f>
+      <c r="B4" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C4" t="s">
@@ -44846,8 +44830,8 @@
       <c r="A5" t="s">
         <v>232</v>
       </c>
-      <c r="B5" s="38" t="str">
-        <f>IF(C5&lt;&gt;A5,"X","")</f>
+      <c r="B5" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C5" t="s">
@@ -44858,8 +44842,8 @@
       <c r="A6" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="38" t="str">
-        <f>IF(C6&lt;&gt;A6,"X","")</f>
+      <c r="B6" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C6" t="s">
@@ -44870,8 +44854,8 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="38" t="str">
-        <f>IF(C7&lt;&gt;A7,"X","")</f>
+      <c r="B7" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C7" t="s">
@@ -44882,8 +44866,8 @@
       <c r="A8" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="38" t="str">
-        <f>IF(C8&lt;&gt;A8,"X","")</f>
+      <c r="B8" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C8" t="s">
@@ -44894,8 +44878,8 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="38" t="str">
-        <f>IF(C9&lt;&gt;A9,"X","")</f>
+      <c r="B9" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C9" t="s">
@@ -44906,8 +44890,8 @@
       <c r="A10" t="s">
         <v>218</v>
       </c>
-      <c r="B10" s="38" t="str">
-        <f>IF(C10&lt;&gt;A10,"X","")</f>
+      <c r="B10" s="32" t="str">
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
     </row>
@@ -44915,8 +44899,8 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="38" t="str">
-        <f>IF(C11&lt;&gt;A11,"X","")</f>
+      <c r="B11" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C11" t="s">
@@ -44927,8 +44911,8 @@
       <c r="A12" t="s">
         <v>224</v>
       </c>
-      <c r="B12" s="38" t="str">
-        <f>IF(C12&lt;&gt;A12,"X","")</f>
+      <c r="B12" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C12" t="s">
@@ -44939,8 +44923,8 @@
       <c r="A13" t="s">
         <v>183</v>
       </c>
-      <c r="B13" s="38" t="str">
-        <f>IF(C13&lt;&gt;A13,"X","")</f>
+      <c r="B13" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C13" t="s">
@@ -44951,8 +44935,8 @@
       <c r="A14" t="s">
         <v>182</v>
       </c>
-      <c r="B14" s="38" t="str">
-        <f>IF(C14&lt;&gt;A14,"X","")</f>
+      <c r="B14" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C14" t="s">
@@ -44963,8 +44947,8 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="38" t="str">
-        <f>IF(C15&lt;&gt;A15,"X","")</f>
+      <c r="B15" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C15" t="s">
@@ -44975,8 +44959,8 @@
       <c r="A16" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="38" t="str">
-        <f>IF(C16&lt;&gt;A16,"X","")</f>
+      <c r="B16" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C16" t="s">
@@ -44987,8 +44971,8 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="38" t="str">
-        <f>IF(C17&lt;&gt;A17,"X","")</f>
+      <c r="B17" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C17" t="s">
@@ -44999,8 +44983,8 @@
       <c r="A18" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="38" t="str">
-        <f>IF(C18&lt;&gt;A18,"X","")</f>
+      <c r="B18" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C18" t="s">
@@ -45011,8 +44995,8 @@
       <c r="A19" t="s">
         <v>189</v>
       </c>
-      <c r="B19" s="38" t="str">
-        <f>IF(C19&lt;&gt;A19,"X","")</f>
+      <c r="B19" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C19" t="s">
@@ -45023,8 +45007,8 @@
       <c r="A20" t="s">
         <v>226</v>
       </c>
-      <c r="B20" s="38" t="str">
-        <f>IF(C20&lt;&gt;A20,"X","")</f>
+      <c r="B20" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C20" t="s">
@@ -45035,8 +45019,8 @@
       <c r="A21" t="s">
         <v>227</v>
       </c>
-      <c r="B21" s="38" t="str">
-        <f>IF(C21&lt;&gt;A21,"X","")</f>
+      <c r="B21" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C21" t="s">
@@ -45047,8 +45031,8 @@
       <c r="A22" t="s">
         <v>228</v>
       </c>
-      <c r="B22" s="38" t="str">
-        <f>IF(C22&lt;&gt;A22,"X","")</f>
+      <c r="B22" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C22" t="s">
@@ -45059,8 +45043,8 @@
       <c r="A23" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="38" t="str">
-        <f>IF(C23&lt;&gt;A23,"X","")</f>
+      <c r="B23" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C23" t="s">
@@ -45071,8 +45055,8 @@
       <c r="A24" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="38" t="str">
-        <f>IF(C24&lt;&gt;A24,"X","")</f>
+      <c r="B24" s="32" t="str">
+        <f t="shared" si="0"/>
         <v>X</v>
       </c>
     </row>
@@ -45080,8 +45064,8 @@
       <c r="A25" t="s">
         <v>162</v>
       </c>
-      <c r="B25" s="38" t="str">
-        <f>IF(C25&lt;&gt;A25,"X","")</f>
+      <c r="B25" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C25" t="s">
@@ -45092,8 +45076,8 @@
       <c r="A26" t="s">
         <v>165</v>
       </c>
-      <c r="B26" s="38" t="str">
-        <f>IF(C26&lt;&gt;A26,"X","")</f>
+      <c r="B26" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C26" t="s">
@@ -45104,8 +45088,8 @@
       <c r="A27" t="s">
         <v>172</v>
       </c>
-      <c r="B27" s="38" t="str">
-        <f>IF(C27&lt;&gt;A27,"X","")</f>
+      <c r="B27" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C27" t="s">
@@ -45116,8 +45100,8 @@
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="38" t="str">
-        <f>IF(C28&lt;&gt;A28,"X","")</f>
+      <c r="B28" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C28" t="s">
@@ -45128,8 +45112,8 @@
       <c r="A29" t="s">
         <v>229</v>
       </c>
-      <c r="B29" s="38" t="str">
-        <f>IF(C29&lt;&gt;A29,"X","")</f>
+      <c r="B29" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C29" t="s">
@@ -45140,8 +45124,8 @@
       <c r="A30" t="s">
         <v>230</v>
       </c>
-      <c r="B30" s="38" t="str">
-        <f>IF(C30&lt;&gt;A30,"X","")</f>
+      <c r="B30" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C30" t="s">
@@ -45152,8 +45136,8 @@
       <c r="A31" t="s">
         <v>231</v>
       </c>
-      <c r="B31" s="38" t="str">
-        <f>IF(C31&lt;&gt;A31,"X","")</f>
+      <c r="B31" s="32" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C31" t="s">
@@ -45165,5 +45149,6 @@
     <sortCondition ref="A2:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit 202512 - pas sûr de quoi mais mise à niveau
</commit_message>
<xml_diff>
--- a/1ere_NSI/z.Progression1NSI_MBR_02.xlsx
+++ b/1ere_NSI/z.Progression1NSI_MBR_02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcbiver/Documents/01_Prof/10_Forge_AEIF/_Forge/1ere_NSI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC80DD9-1118-9641-B0A5-02D5610CEA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6633C9-D9B9-7C41-ACD6-7BB66C401995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProgressionMBR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ProgressionMBR_PRINT!$A$1:$E$46</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">ProgressionMBR_PRINT!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="255">
   <si>
     <t>Elt Prog</t>
   </si>
@@ -966,6 +966,137 @@
   <si>
     <t>Web</t>
   </si>
+  <si>
+    <t>Travaux pratiques - Sur un fichier de l'INSEE (données de tous les lycées de France pour la rentrée 2022), réalisation de traitements de données divers - recherche d'éléments, comptage suivant un filtre, statistiques diverses. Introduction par ce biais à la notion d'algorithme.
+Pour le 2/2:
+Activité de traitement des données de lycée à la rentrée 2022 (dans Capitale v2, code a8fb-2861201 pour ceux qui ne l'ont pas commencée) - tout compléter jusqu'à la fin de la question 4 ("Docteur Dupont").
+Pour le 30/1:
+Rappel: soumission avant mardi soir de la V2 de vos documents de projet sur l'espace documentaire de l'ENT.
+Travaux pratiques - Traitement de données d'un fichier CSV
+Suite du TP sur un fichier de l'INSEE (données de tous les lycées de France pour la rentrée 2022), réalisation de traitements de données divers - recherche d'éléments, comptage suivant un filtre, statistiques diverses. Introduction par ce biais à la notion d'algorithme.
+Flash quiz 02
+Pour le 9/2:
+Poursuite des activités sur le fichier des données de LV dans les lycées français: compléter TOUTES les questions jusqu'à la 7.1 incluse. ATTENTION: pour rappel, cette activité sera notée...</t>
+  </si>
+  <si>
+    <t>Activité de groupe - Travail sur les projets
+En binômes, séance consacrée à l'avancement de notre première série de projets.
+Cours - Présentation ChatGPT
+Hors programme: présentation de l'AI et spécifiquement de ChatGPT: fonctionnement, principes d'utilisation, conseils pour la rédaction de prompts.</t>
+  </si>
+  <si>
+    <t>Cours + TD - Introduction à l'algorithmique
+Présentation du sujet, mise dans le contexte du programme de l'année dans son ensemble; spécification d'algorithme, rédaction traitement des données en pseudo-code.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: traduction d'algorithmes en Python, tests d'algorithmes, variants de boucle pour prouver la terminaison.</t>
+  </si>
+  <si>
+    <t>Activité de groupe - Travail sur les projets
+En binômes, séance consacrée à l'avancement de notre première série de projets.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: invariants de boucle.
+Pour le 8/3:
+Exercices 2, 3, et 4 du cahier d'exercices d'entraînement à l'algorithmique que vous trouverez en ligne dans notre espace documentaire partagé de l'ENT, dans le répertoire "1NSIGr2 / COURS / 06_Algorithmique" (je le joins ici aussi à tout hasard).
+Pour le 11/3:
+Réaliser l'avancement de votre projet selon les objectifs que je vous ai envoyés par mail vendredi soir. MERCI DE ME REMETTRE VOTRE TRAVAIL DIMANCHE SOIR (par mail ou en le soumettant sur l'espace documentaire, comme vous préférez) pour que je puisse en prendre connaissance lundi matin et qu'on ne perde pas de temps pendant le cours. Merci et bon courage!
+Cours + TD - Introduction à l'algorithmique
+Suite du chapitre - fin invariants de boucle, intro algorithmes de tri, tri par permutations (tri à bulles).
+Pour le 11/3:
+Exercices 5, 6, et 7 du cahier d'exercices d'entraînement à l'algorithmique que vous trouverez en ligne dans notre espace documentaire partagé de l'ENT, dans le répertoire "1NSIGr2 / COURS / 06_Algorithmique" (je le joins ici aussi à tout hasard).</t>
+  </si>
+  <si>
+    <t>Activité de groupe - Travail sur les projets
+En binômes, séance consacrée à l'avancement de notre première série de projets.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin tri à bulles, tri par sélection.
+Pour le 15/3:
+Exercice 8 du cahier d'exercices algorithmique que j'ai partagé dans l'espace documentaire ENT à faire - on le corrigera en séance vendredi.
+Pour le 18/3:
+Réaliser l'avancement de votre projet selon les objectifs que je vous ai envoyés par mail vendredi soir. MERCI DE ME REMETTRE VOTRE TRAVAIL DIMANCHE SOIR (par mail ou en le soumettant sur l'espace documentaire, comme vous préférez) pour que je puisse en prendre connaissance lundi matin et qu'on ne perde pas de temps pendant le cours. Merci et bon courage!
+Pour le 5/4:
+Soumission de votre projet #1 terminé (au sens des objectifs que je vous ai fixés par mail cette semaine). Je les reverrai pendant les vacances et ils feront tous l'objet d'une présentation / démonstration par vous à la classe entière à la rentrée.
+Comme d'habitude, la soumission doit être faite sous la forme d'un fichier Python (plus éventuellement des fichiers annexes selon la nature de votre projet), à m'envoyer:
+- Soit par le mail de l'ENT;
+- Soit sur mon mail académique (marc.biver@ac-versailles.fr)
+- Soit sur l'espace partagé que l'on a créé sur l'ENT pour votre projet.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin tri par sélection; tri par insertion.
+Flash quiz 04</t>
+  </si>
+  <si>
+    <t>Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin tri par insertion, comparaisons performances et caractéristiques des trois types de tri vus en séance.
+Flash quiz 04 (fin)
+Pour le 22/3:
+Activités page 36 du cours en ligne sur l'ENT (01_CoursAlgorithmique_v0.3.pdf): exercices 16, 17, et 18 à vérifier / compléter (on les a faits en cours) + rédaction du pseudo-code de l'algorithme de recherche dichotomique. Ces trois activités sont à faire sur feuille et je les relèverai.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin des tris, début algorithmes de recherche (séquentielle, dichotomique).
+Activité de groupe - Travail sur les projets
+En binômes, séance consacrée à l'avancement de notre première série de projets.
+Pour le 25/3:
+A rendre lundi: exercices 10 et 11 du cahier d'exercices qui est sur l'ENT (dans le répertoire Algorithmique). Ce sera relevé. En cas de problème / question je vous rappelle mon adresse académique: marc.biver@ac-versailles.fr</t>
+  </si>
+  <si>
+    <t>Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin recherche dichotomique, algorithmes gloutons.
+Cours + TD - Introduction à l'algorithmique
+Suite de la thématique: fin algorithmes gloutons.
+Activité de groupe - Projets, série #2
+Choix des thèmes pour le second projet. [CES PROJETS N'ONT PAS ETE REALISES FAUTE DE TEMPS]
+Révisions - Révisions en vue du contrôle du 5/4
+Exercices d'entraînement, revue des concepts potentiellement peu clairs.</t>
+  </si>
+  <si>
+    <t>Devoir sur table - Devoir majeur #4
+Contrôle portant sur tout ce que nous avons fait en algorithmique (jusqu'aux algorithmes gloutons inclus) ainsi que sur le traitement de données en table (manipulation de fichiers CSV, dictionnaires...). Il est évident que vous aurez aussi besoin de votre maîtrise du Python. Les autres sujets (web, architecture physique, représentation des données) ne sont en revanche pas au programme.
+Les outils à votre disposition pour réviser sont:
+- Le cours d'algorithmique qui est en ligne (dernière version = 0.4): maitrisez parfaitement tous les exercices qu'il comporte (toutes les corrections sont incluses) et faites attention aux encadrés "A Savoir / A Réviser";
+- Le cahier d'exercices d'algo / traitement de données en table (dernière version = 0.3) avec corrections: vous devez tous les maitriser parce que ceux du contrôle seront très similaires;
+- Les quiz / corrections qu'on a fait en cours;
+- Les aide-mémoires que je vous ai fournis pour le traitement des données en table (un sur les fichiers, un sur les dictionnaires). Il n'est pas nécessaire de connaitre par coeur la syntaxe du module CSV - juste être capable de la lire et de manipuler les objets (comme des listes de dictionnaires) qui en découlent.
+BON COURAGE A TOUS!
+Cours - Introduction à Pygame
+Présentation du document joint et premiers exemples de code s'appuyant sur pygame (fenêtre vide; avec une image d'un ballon statique; déplacement du ballon; rebond du ballon sur les bords de la fenêtre).
+L'exercice 1 (au moins - les 2 et 3 sont optionnels) de la dernière partie du document est à faire pour la rentrée.
+Pour le 26/4:
+Parcourir le document d'introduction à Pygame (présent dans l'espace documentaire partagé de l'ENT et également joint au cahier de textes de notre cours du 05/04) et réaliser le code de l'exercice 1 (de la partie 6 du document). A me remettre par mail. IMPORTANT: je le mets pour le vendredi de la rentrée pour que si vous avez été bloqués pendant les vacances vous puissiez venir me voir lundi. Donc il faut absolument que vous testiez pygame sur votre ordinateur pendant les vacances.</t>
+  </si>
+  <si>
+    <t>Cours + TD - Introduction au thème Architecture Système
+Introduction aux niveaux de langages puis au langage assembleur. TD en séance sur le simulateur de Peter Higginson.
+Pour le 26/4:
+Me soumettre par mail / casier ENT un document comportant les réponses à l'exercice 1 sur le langage assembleur - vous le trouverez dans le document que je viens de mettre en ligne sur notre espace documentaire sur l'ENT (nouveau répertoire dans "COURS" appelé "07_ArchitectureSystème").
+Cours + TD - Architecture système - suite
+Suite de la séance précédente - exercices du cours dans le simulateur.</t>
+  </si>
+  <si>
+    <t>Cours + TD - Architecture système - suite
+Enchainement sur les systèmes d'exploitation: TP sur Terminus et début du TP sur Shell directement.</t>
+  </si>
+  <si>
+    <t>Cours + TD - Architecture système - suite
+Correction du TP sur Shell puis introduction aux réseaux: présentation / rappels de SNT, puis vidéo accompagnée d'un questionnaire à rendre.
+Pour le 13/5:
+Exercice 3 du TP "02_TP2_Shell" à faire sur papier et à remettre. Le document est disponible dans COURS / 07_ArchitectureSysteme.
+Pour le 13/5:
+Questionnaire d'introduction sur les réseaux à compléter et à remettre. Le document (nommé "20240506_NSI_QuestionnaireIntroReseaux") est disponible dans COURS / 07_ArchitectureSysteme. Les vidéos à visionner sont en lien dans le document (la première est celle qu'on a vue en séance aujourd'hui).</t>
+  </si>
+  <si>
+    <t>Cours + TD - Architecture système - suite
+S'appuyant sur le questionnaire réalisé sur la base des vidéos, cours sur les réseaux: histoire, protocoles, TCP/IP, masques de sous-réseau... Réalisation d'exercices en vue du contrôle de la semaine prochaine.
+Pour le 17/5:
+Exercices 4 et 5 du fichier "02.Reseaux_cours_exercices" présent dans l'espace documentaire partagé de l'ENT (dans le zip "CoursActivitesReseaux" du répertoire "Architecture Système").
+Pour le 17/5:
+Préparation (en binôme) d'une brève présentation en classe de votre projet #1. Elle durera 5 minutes: une démonstration de l'exécution de votre programme et l'explication d'une de ses fonctions qu'on affichera - son algorithme (entrées / sorties / traitement) et sa syntaxe (utilisation de boucles, de structures conditionnelles...).  J'enverrai à chaque groupe un mail Mercredi spécifiant exactement quelle fonction je  suggère, mais ce ne sera qu'une suggestion: s'il y en a une que vous trouvez particulièrement complexe ou intéressante, vous pouvez tout à fait la choisir et donc commencer dès à présent à préparer sa présentation. Bon courage et à vendredi!
+Activité de groupe - Présentation des projets
+6 groupes sur 11 ont présenté le fruit de leur projet: explication du cahier des charges à la classe, exécution / démo du code, discussion de l'approche de programmation (algorithme, structures de données, etc.)
+Travaux dirigés - Architecture système - suite
+Feuille d'exercices représentatifs de ce qui sera au contrôle de la semaine prochaine: réalisation en séance de deux d'entre eux. La correction des autres a été mise en ligne sur l'espace documentaire de l'ENT le 20/05.</t>
+  </si>
+  <si>
+    <t>Devoir Majeur - Architecture Système
+Dernier devoir majeur de l'année sur les thèmes vus depuis les vacances de Printemps - assembleur, OS, réseau…</t>
+  </si>
 </sst>
 </file>
 
@@ -1115,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1210,6 +1341,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1475,9 +1609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XEV45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.19921875" defaultRowHeight="14" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -18103,7 +18237,7 @@
       <c r="AMC22" s="19"/>
       <c r="AMD22" s="19"/>
     </row>
-    <row r="23" spans="1:1018 16375:16376" s="7" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1018 16375:16376" s="7" customFormat="1" ht="225" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10">
         <v>45320</v>
       </c>
@@ -18119,11 +18253,13 @@
       <c r="E23" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="33" t="s">
+        <v>242</v>
+      </c>
       <c r="XEU23" s="19"/>
       <c r="XEV23" s="19"/>
     </row>
-    <row r="24" spans="1:1018 16375:16376" s="7" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1018 16375:16376" s="7" customFormat="1" ht="75" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10">
         <v>45327</v>
       </c>
@@ -18139,7 +18275,9 @@
       <c r="E24" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="33" t="s">
+        <v>243</v>
+      </c>
       <c r="XEU24" s="19"/>
       <c r="XEV24" s="19"/>
     </row>
@@ -20191,7 +20329,7 @@
       <c r="AMC26" s="19"/>
       <c r="AMD26" s="19"/>
     </row>
-    <row r="27" spans="1:1018 16375:16376" s="7" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1018 16375:16376" s="7" customFormat="1" ht="75" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10">
         <v>45348</v>
       </c>
@@ -20207,11 +20345,13 @@
       <c r="E27" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="33" t="s">
+        <v>244</v>
+      </c>
       <c r="XEU27" s="19"/>
       <c r="XEV27" s="19"/>
     </row>
-    <row r="28" spans="1:1018 16375:16376" s="7" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1018 16375:16376" s="7" customFormat="1" ht="255" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10">
         <v>45355</v>
       </c>
@@ -20227,11 +20367,13 @@
       <c r="E28" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="33" t="s">
+        <v>245</v>
+      </c>
       <c r="XEU28" s="19"/>
       <c r="XEV28" s="19"/>
     </row>
-    <row r="29" spans="1:1018 16375:16376" s="7" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1018 16375:16376" s="7" customFormat="1" ht="314" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10">
         <v>45362</v>
       </c>
@@ -20247,11 +20389,13 @@
       <c r="E29" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="33" t="s">
+        <v>246</v>
+      </c>
       <c r="XEU29" s="19"/>
       <c r="XEV29" s="19"/>
     </row>
-    <row r="30" spans="1:1018 16375:16376" s="7" customFormat="1" ht="60" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1018 16375:16376" s="7" customFormat="1" ht="210" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10">
         <v>45369</v>
       </c>
@@ -20267,11 +20411,13 @@
       <c r="E30" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="F30" s="6"/>
+      <c r="F30" s="33" t="s">
+        <v>247</v>
+      </c>
       <c r="XEU30" s="19"/>
       <c r="XEV30" s="19"/>
     </row>
-    <row r="31" spans="1:1018 16375:16376" s="7" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1018 16375:16376" s="7" customFormat="1" ht="135" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10">
         <v>45376</v>
       </c>
@@ -20287,11 +20433,13 @@
       <c r="E31" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="33" t="s">
+        <v>248</v>
+      </c>
       <c r="XEU31" s="19"/>
       <c r="XEV31" s="19"/>
     </row>
-    <row r="32" spans="1:1018 16375:16376" s="7" customFormat="1" ht="15" outlineLevel="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1018 16375:16376" s="7" customFormat="1" ht="328" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10">
         <v>45383</v>
       </c>
@@ -20307,7 +20455,9 @@
       <c r="E32" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="F32" s="6"/>
+      <c r="F32" s="33" t="s">
+        <v>249</v>
+      </c>
       <c r="XEU32" s="19"/>
       <c r="XEV32" s="19"/>
     </row>
@@ -22359,7 +22509,7 @@
       <c r="AMC34" s="19"/>
       <c r="AMD34" s="19"/>
     </row>
-    <row r="35" spans="1:1018" s="7" customFormat="1" ht="75" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1018" s="7" customFormat="1" ht="120" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A35" s="10">
         <v>45404</v>
       </c>
@@ -22375,7 +22525,9 @@
       <c r="E35" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="F35" s="6"/>
+      <c r="F35" s="33" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="36" spans="1:1018" s="7" customFormat="1" ht="45" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A36" s="10">
@@ -22393,9 +22545,11 @@
       <c r="E36" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="33" t="s">
+        <v>251</v>
+      </c>
     </row>
-    <row r="37" spans="1:1018" s="7" customFormat="1" ht="45" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1018" s="7" customFormat="1" ht="105" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A37" s="10">
         <v>45418</v>
       </c>
@@ -22411,9 +22565,11 @@
       <c r="E37" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="F37" s="6"/>
+      <c r="F37" s="33" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="38" spans="1:1018" s="7" customFormat="1" ht="15" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1018" s="7" customFormat="1" ht="270" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A38" s="10">
         <v>45425</v>
       </c>
@@ -22429,9 +22585,11 @@
       <c r="E38" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="33" t="s">
+        <v>253</v>
+      </c>
     </row>
-    <row r="39" spans="1:1018" s="7" customFormat="1" ht="15" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1018" s="7" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A39" s="10">
         <v>45432</v>
       </c>
@@ -22447,25 +22605,27 @@
       <c r="E39" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="F39" s="6"/>
+      <c r="F39" s="33" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="40" spans="1:1018" s="7" customFormat="1" ht="30" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="A40" s="10">
+      <c r="A40" s="13">
         <v>45439</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="14">
         <v>39</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:1018" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13">
@@ -23677,7 +23837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC8AD568-4811-1342-9396-688F6B1D2247}">
   <dimension ref="A1:XEU45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>

</xml_diff>